<commit_message>
Update schedule file: Y4_B2526_Pediatrics_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y4_B2526_Pediatrics_schedule.xlsx
+++ b/modules_schedules/Y4_B2526_Pediatrics_schedule.xlsx
@@ -69,7 +69,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -84,18 +84,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -463,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,7 +513,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>PED-A1-1</t>
+          <t>PED-B1-5</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -540,156 +528,16 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>10/09/2025</t>
+          <t>11/09/2025</t>
         </is>
       </c>
       <c r="F2" s="4" t="inlineStr">
         <is>
-          <t>10:00:00</t>
+          <t>08:00:00</t>
         </is>
       </c>
       <c r="G2" s="5" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>PED-A1-1</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>pediatrics</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E3" s="7" t="inlineStr">
-        <is>
-          <t>11/09/2025</t>
-        </is>
-      </c>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>10:00:00</t>
-        </is>
-      </c>
-      <c r="G3" s="9" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>PED-A1-1</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>pediatrics</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>16/09/2025</t>
-        </is>
-      </c>
-      <c r="F4" s="4" t="inlineStr">
-        <is>
-          <t>10:00:00</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B5" s="6" t="inlineStr">
-        <is>
-          <t>PED-A1-1</t>
-        </is>
-      </c>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>pediatrics</t>
-        </is>
-      </c>
-      <c r="D5" s="6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>17/09/2025</t>
-        </is>
-      </c>
-      <c r="F5" s="8" t="inlineStr">
-        <is>
-          <t>10:00:00</t>
-        </is>
-      </c>
-      <c r="G5" s="9" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>PED-A1-1</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>pediatrics</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>18/09/2025</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="inlineStr">
-        <is>
-          <t>10:00:00</t>
-        </is>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>180</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>